<commit_message>
Update v2 unit test
</commit_message>
<xml_diff>
--- a/IntegrationPlanning_v1.xlsx
+++ b/IntegrationPlanning_v1.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doanthithuy/Documents/Live Poroject Guru99/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E3BBA0-65CB-774E-A653-4B2A6BBD4A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="ChangeLog" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="IntegrationPlanning" sheetId="2" r:id="rId4"/>
+    <sheet name="ChangeLog" sheetId="1" r:id="rId1"/>
+    <sheet name="IntegrationPlanning" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -24,9 +33,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>15/11/2013</t>
   </si>
   <si>
     <t>Harick</t>
@@ -320,38 +326,42 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Verdana"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -361,7 +371,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -389,16 +399,30 @@
     </fill>
   </fills>
   <borders count="6">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -413,181 +437,486 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B1:G99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="30.38"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
         <v>0</v>
@@ -603,592 +932,593 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12">
+    <row r="12" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5"/>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="21">
+        <v>44880</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>6</v>
-      </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13">
+    <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36">
+    <row r="36" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37">
+    <row r="37" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39">
+    <row r="39" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40">
+    <row r="40" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44">
+    <row r="44" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46">
+    <row r="46" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47">
+    <row r="47" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48">
+    <row r="48" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50">
+    <row r="50" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51">
+    <row r="51" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52">
+    <row r="52" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53">
+    <row r="53" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54">
+    <row r="54" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55">
+    <row r="55" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56">
+    <row r="56" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59">
+    <row r="59" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60">
+    <row r="60" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61">
+    <row r="61" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62">
+    <row r="62" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63">
+    <row r="63" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64">
+    <row r="64" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66">
+    <row r="66" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68">
+    <row r="68" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69">
+    <row r="69" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70">
+    <row r="70" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71">
+    <row r="71" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72">
+    <row r="72" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73">
+    <row r="73" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74">
+    <row r="74" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75">
+    <row r="75" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76">
+    <row r="76" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77">
+    <row r="77" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78">
+    <row r="78" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79">
+    <row r="79" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80">
+    <row r="80" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81">
+    <row r="81" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82">
+    <row r="82" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83">
+    <row r="83" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84">
+    <row r="84" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85">
+    <row r="85" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86">
+    <row r="86" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87">
+    <row r="87" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88">
+    <row r="88" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89">
+    <row r="89" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90">
+    <row r="90" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91">
+    <row r="91" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92">
+    <row r="92" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93">
+    <row r="93" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94">
+    <row r="94" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95">
+    <row r="95" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96">
+    <row r="96" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97">
+    <row r="97" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98">
+    <row r="98" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99">
+    <row r="99" spans="3:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.88"/>
-    <col customWidth="1" min="5" max="5" width="29.25"/>
-    <col customWidth="1" min="6" max="6" width="27.63"/>
-    <col customWidth="1" min="7" max="7" width="28.88"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -1203,581 +1533,581 @@
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="H3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="17" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="17" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="17" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="17" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18" t="s">
+      <c r="D13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="G13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="18" t="s">
+      <c r="D14" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18" t="s">
+      <c r="D15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="E15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="F15" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="G15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="F16" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="G16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18" t="s">
+      <c r="D17" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="G17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="D18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="G18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="F19" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>27</v>
+      <c r="G19" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
+        <v>21</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update v1 unit test
</commit_message>
<xml_diff>
--- a/IntegrationPlanning_v1.xlsx
+++ b/IntegrationPlanning_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doanthithuy/Documents/Live Poroject Guru99/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E3BBA0-65CB-774E-A653-4B2A6BBD4A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE0B0C-88B2-584B-BBE1-554E0ECB4CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeLog" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Harick</t>
-  </si>
-  <si>
     <t>Initial Draft</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t xml:space="preserve">Display Generated Customized statement </t>
+  </si>
+  <si>
+    <t>Đoàn Thị Thuý</t>
   </si>
 </sst>
 </file>
@@ -336,34 +336,41 @@
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -847,12 +854,13 @@
   </sheetPr>
   <dimension ref="B1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -941,10 +949,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>5</v>
       </c>
       <c r="G12" s="8"/>
     </row>
@@ -1482,8 +1490,8 @@
   </sheetPr>
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1495,30 +1503,30 @@
     <col min="7" max="7" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -1535,28 +1543,28 @@
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>21</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -1566,28 +1574,28 @@
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="228" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -1597,30 +1605,30 @@
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="228" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>30</v>
-      </c>
       <c r="G4" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -1630,28 +1638,28 @@
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="171" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -1661,28 +1669,28 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>39</v>
-      </c>
       <c r="G6" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
@@ -1692,30 +1700,30 @@
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -1725,28 +1733,28 @@
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="114" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="G8" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -1756,28 +1764,28 @@
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="G9" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1787,30 +1795,30 @@
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="G10" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -1820,28 +1828,28 @@
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="G11" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -1851,30 +1859,30 @@
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>65</v>
-      </c>
       <c r="G12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -1884,28 +1892,28 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="G13" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
@@ -1915,28 +1923,28 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="76" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -1946,28 +1954,28 @@
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="95" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="E15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="F15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>75</v>
-      </c>
       <c r="G15" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -1977,30 +1985,30 @@
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="F16" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="G16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -2010,28 +2018,28 @@
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="95" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="G17" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -2041,30 +2049,30 @@
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="76" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="D18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>87</v>
-      </c>
       <c r="G18" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
@@ -2074,30 +2082,30 @@
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="76" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="C19" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="D19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="G19" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>

</xml_diff>